<commit_message>
Biofuel ICE option added
</commit_message>
<xml_diff>
--- a/MicroGrids/Results/Battery_Data.xlsx
+++ b/MicroGrids/Results/Battery_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\Desktop\MicroGridsPy-Teaching\MicroGridsPy-Teaching-multi-year-capacity-expansion-MYCE-\MicroGrids\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6CB7B0F-2BBC-46F1-8D6E-4C955C4EB0B2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B59D0E66-FB58-41B3-B898-65334048190F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3240" yWindow="3240" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Battery_Data" sheetId="1" r:id="rId1"/>
@@ -32,16 +32,16 @@
     <t>Yearly O&amp;M Cost at upgrade 1</t>
   </si>
   <si>
-    <t>Total actualized Battery Reposition Cost</t>
+    <t>Total actualized Battery Replacement Cost</t>
   </si>
   <si>
     <t>Scenario 1</t>
   </si>
   <si>
-    <t>Battery Reposition Cost at y = 1</t>
-  </si>
-  <si>
-    <t>Battery Reposition Cost at y = 2</t>
+    <t>Battery Replacement Cost at y = 1</t>
+  </si>
+  <si>
+    <t>Battery Replacement Cost at y = 2</t>
   </si>
 </sst>
 </file>
@@ -449,7 +449,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -463,7 +463,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>499086.75462399999</v>
+        <v>508909.30501200003</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -471,7 +471,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>369324.19842176</v>
+        <v>376592.88570888003</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -479,7 +479,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>7386.4839684352</v>
+        <v>7531.8577141776004</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -487,7 +487,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>49496.317985000001</v>
+        <v>50418.5832974</v>
       </c>
     </row>
   </sheetData>
@@ -503,7 +503,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -517,7 +517,7 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>24743.356259290631</v>
+        <v>25202.447014969581</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -525,7 +525,7 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>24752.961725752371</v>
+        <v>25216.136282408941</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added BarHomogeneous to gurobi solver
</commit_message>
<xml_diff>
--- a/MicroGrids/Results/Battery_Data.xlsx
+++ b/MicroGrids/Results/Battery_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\Desktop\MicroGridsPy-Teaching\MicroGridsPy-Teaching-multi-year-capacity-expansion-MYCE-\MicroGrids\Results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Giulia\GitHub\MicroGridsPy-Teaching\MicroGrids\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B59D0E66-FB58-41B3-B898-65334048190F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBFEB9CA-558D-47E6-8E61-BA535A2EAB45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Battery_Data" sheetId="1" r:id="rId1"/>
@@ -447,47 +447,47 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>508909.30501200003</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>0.53158528266100002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>376592.88570888003</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+        <v>0.39337310916913998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>7531.8577141776004</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+        <v>7.8674621833828007E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>50418.5832974</v>
+        <v>0.113355856262</v>
       </c>
     </row>
   </sheetData>
@@ -501,31 +501,31 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B2">
-        <v>25202.447014969581</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>5.668131650166288E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B3">
-        <v>25216.136282408941</v>
+        <v>5.6674539760673173E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>